<commit_message>
renamed cut_before and cut_after to cut_ends and cut_beginnings
</commit_message>
<xml_diff>
--- a/specific_options_examples.xlsx
+++ b/specific_options_examples.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\zip\FFR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\zip\FFR\ffr_analysis\sort_ffr_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -97,21 +97,9 @@
     <t>steepest</t>
   </si>
   <si>
-    <t>cut_after</t>
-  </si>
-  <si>
-    <t>cut_after is the number seconds of data which are cut out after a switch between chambers</t>
-  </si>
-  <si>
-    <t>cut_before is the number of seconds of data which are cut out before a switch between chambers</t>
-  </si>
-  <si>
     <t>A heading like left:CO2:start means the regression will start at that time for CO2 on left side</t>
   </si>
   <si>
-    <t>cut_before and cut_after may not be side or substance or side specific (so N2O:cut_before or left:cut_before is not allowed)</t>
-  </si>
-  <si>
     <t>2017-12-09-13-19-30-x599229_657278-y6615153_90987-z0_0-h0_727911466692_right_Plot_6_</t>
   </si>
   <si>
@@ -128,6 +116,18 @@
   </si>
   <si>
     <t>2017-12-09-13-42-16-x599275_970756-y6615195_76834-z0_0-h0_734873089817_right_Plot_11_</t>
+  </si>
+  <si>
+    <t>cut_beginnings is the number seconds of data which are cut out after a switch between chambers</t>
+  </si>
+  <si>
+    <t>cut_ends is the number of seconds of data which are cut out before a switch between chambers</t>
+  </si>
+  <si>
+    <t>cut_beginnings and cut_ends may not be side or substance or side specific (so N2O:cut_ends or left:cut_ends is not allowed)</t>
+  </si>
+  <si>
+    <t>cut_beginnings</t>
   </si>
 </sst>
 </file>
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -475,7 +475,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -495,17 +495,17 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -557,7 +557,7 @@
         <v>20</v>
       </c>
       <c r="O13" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -565,7 +565,7 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -579,7 +579,7 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C15">
         <v>100</v>
@@ -593,7 +593,7 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C16">
         <v>100</v>
@@ -616,7 +616,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C17">
         <v>100</v>
@@ -642,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C18">
         <v>100</v>
@@ -659,7 +659,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>